<commit_message>
Failed to figure out reorder row issue
</commit_message>
<xml_diff>
--- a/Output/exported.xlsx
+++ b/Output/exported.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t>Day</t>
   </si>
@@ -34,31 +34,40 @@
     <t>Friday</t>
   </si>
   <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>9:30am - 10:45am</t>
+  </si>
+  <si>
+    <t>8:00pm - 9:15pm</t>
+  </si>
+  <si>
     <t>8:00am - 9:15am</t>
   </si>
   <si>
-    <t>9:30am - 10:45am</t>
+    <t>6:30pm - 7:45pm</t>
+  </si>
+  <si>
+    <t>5:00pm - 6:15pm</t>
+  </si>
+  <si>
+    <t>3:30pm - 4:45pm</t>
+  </si>
+  <si>
+    <t>2:00pm - 3:15pm</t>
+  </si>
+  <si>
+    <t>12:30pm - 1:45pm</t>
   </si>
   <si>
     <t>11:00am - 12:15pm</t>
   </si>
   <si>
-    <t>12:30pm - 1:45pm</t>
-  </si>
-  <si>
-    <t>2:00pm - 3:15pm</t>
-  </si>
-  <si>
-    <t>3:30pm - 4:45pm</t>
-  </si>
-  <si>
-    <t>5:00pm - 6:15pm</t>
-  </si>
-  <si>
-    <t>6:30pm - 7:45pm</t>
-  </si>
-  <si>
-    <t>8:00pm - 9:15pm</t>
+    <t>Student Scheduler</t>
+  </si>
+  <si>
+    <t>AVAILABLE</t>
   </si>
 </sst>
 </file>
@@ -416,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -443,48 +452,233 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried a few more tactics to sort by columns
</commit_message>
<xml_diff>
--- a/Output/exported.xlsx
+++ b/Output/exported.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>Day</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Friday</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>9:30am - 10:45am</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>11:00am - 12:15pm</t>
-  </si>
-  <si>
-    <t>Student Scheduler</t>
   </si>
   <si>
     <t>AVAILABLE</t>
@@ -425,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,231 +447,208 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="G10">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got reordering of rows working
</commit_message>
<xml_diff>
--- a/Output/exported.xlsx
+++ b/Output/exported.xlsx
@@ -34,31 +34,31 @@
     <t>Friday</t>
   </si>
   <si>
+    <t>8:00am - 9:15am</t>
+  </si>
+  <si>
     <t>9:30am - 10:45am</t>
   </si>
   <si>
+    <t>11:00am - 12:15pm</t>
+  </si>
+  <si>
+    <t>12:30pm - 1:45pm</t>
+  </si>
+  <si>
+    <t>2:00pm - 3:15pm</t>
+  </si>
+  <si>
+    <t>3:30pm - 4:45pm</t>
+  </si>
+  <si>
+    <t>5:00pm - 6:15pm</t>
+  </si>
+  <si>
+    <t>6:30pm - 7:45pm</t>
+  </si>
+  <si>
     <t>8:00pm - 9:15pm</t>
-  </si>
-  <si>
-    <t>8:00am - 9:15am</t>
-  </si>
-  <si>
-    <t>6:30pm - 7:45pm</t>
-  </si>
-  <si>
-    <t>5:00pm - 6:15pm</t>
-  </si>
-  <si>
-    <t>3:30pm - 4:45pm</t>
-  </si>
-  <si>
-    <t>2:00pm - 3:15pm</t>
-  </si>
-  <si>
-    <t>12:30pm - 1:45pm</t>
-  </si>
-  <si>
-    <t>11:00am - 12:15pm</t>
   </si>
   <si>
     <t>AVAILABLE</t>
@@ -447,91 +447,91 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
+      <c r="C4">
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="C5">
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
       </c>
       <c r="G5" t="s">
         <v>15</v>
@@ -539,16 +539,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
+      <c r="C6">
         <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -585,16 +585,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
         <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -608,22 +608,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
-        <v>4</v>
+      <c r="C9" t="s">
+        <v>15</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
       </c>
       <c r="G9" t="s">
         <v>15</v>
@@ -631,25 +631,25 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
-        <v>3</v>
+      <c r="C10" t="s">
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>9</v>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>